<commit_message>
updated dataset with gvwr and advanced segment classifications
</commit_message>
<xml_diff>
--- a/Truck Segment Classification.xlsx
+++ b/Truck Segment Classification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://calstartcompany-my.sharepoint.com/personal/blatif_calstart_org/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/basillatif/Desktop/CALSTART.nosync/Super_Portal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19E477B5-04A3-4B4F-A4F9-1A7944C7ADA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD508A7-111D-8441-AFBF-F8539C9A2FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21600" windowHeight="18960" xr2:uid="{9086D82A-EACB-9740-B175-4E84EF38D0E6}"/>
+    <workbookView xWindow="-38400" yWindow="11380" windowWidth="38400" windowHeight="21100" xr2:uid="{9086D82A-EACB-9740-B175-4E84EF38D0E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="71">
   <si>
     <t>HVIP Segments</t>
   </si>
@@ -224,9 +224,6 @@
     <t>Notes About Data</t>
   </si>
   <si>
-    <t>if GVWR &lt;= 2600:</t>
-  </si>
-  <si>
     <t>if GVWR == 26001-33000 OR GVWR == &gt;33000:</t>
   </si>
   <si>
@@ -258,13 +255,34 @@
   </si>
   <si>
     <t xml:space="preserve">else == </t>
+  </si>
+  <si>
+    <t>if GVWR &lt;= 26000:</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Count Utility Trucks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID Drayage </t>
+  </si>
+  <si>
+    <t>Class 6 Box Truck</t>
+  </si>
+  <si>
+    <t>Look at fleet name behind Transit/Shuttle Bus category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change coach to charter </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -366,7 +384,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -381,6 +399,7 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,34 +733,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B152D04-ACEC-6549-86A6-E55C740C65FB}">
   <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J24" activeCellId="1" sqref="J42 J24"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.875" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" customWidth="1"/>
     <col min="9" max="10" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.875" customWidth="1"/>
-    <col min="15" max="15" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
@@ -781,7 +800,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -825,7 +844,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
@@ -858,7 +877,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -884,7 +903,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
@@ -907,7 +926,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -927,7 +946,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -938,7 +957,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -955,7 +974,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -966,7 +985,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -980,7 +999,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>25</v>
       </c>
@@ -994,7 +1013,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>36</v>
       </c>
@@ -1008,7 +1027,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
@@ -1022,7 +1041,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>34</v>
       </c>
@@ -1033,7 +1052,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
@@ -1044,7 +1063,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>27</v>
       </c>
@@ -1055,7 +1074,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>35</v>
       </c>
@@ -1066,7 +1085,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>40</v>
       </c>
@@ -1077,7 +1096,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
@@ -1088,7 +1107,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>31</v>
       </c>
@@ -1099,55 +1118,55 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D23" t="s">
+        <v>64</v>
+      </c>
+      <c r="I23" t="s">
         <v>53</v>
       </c>
-      <c r="I23" t="s">
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" ht="15.75">
-      <c r="A24" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>19</v>
       </c>
       <c r="F24" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" t="s">
         <v>57</v>
       </c>
-      <c r="G24" t="s">
-        <v>58</v>
-      </c>
       <c r="I24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J24" s="6" t="s">
         <v>17</v>
       </c>
       <c r="K24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E25" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E26" s="10" t="s">
         <v>35</v>
       </c>
@@ -1155,7 +1174,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>65</v>
+      </c>
       <c r="E27" s="10" t="s">
         <v>28</v>
       </c>
@@ -1163,7 +1185,10 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>66</v>
+      </c>
       <c r="E28" s="10" t="s">
         <v>40</v>
       </c>
@@ -1171,7 +1196,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
       <c r="E29" s="10" t="s">
         <v>42</v>
       </c>
@@ -1179,261 +1207,270 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>69</v>
+      </c>
       <c r="J30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>70</v>
+      </c>
       <c r="D31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E31" t="s">
         <v>18</v>
       </c>
       <c r="F31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G31" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J32" t="s">
         <v>18</v>
       </c>
       <c r="K32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L32" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="4:12">
+    <row r="33" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E33" t="s">
         <v>17</v>
       </c>
       <c r="F33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G33" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="4:12">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="4:12" x14ac:dyDescent="0.2">
       <c r="I34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J34" s="7" t="s">
         <v>25</v>
       </c>
       <c r="K34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L34" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="4:12">
+    <row r="35" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E35" t="s">
         <v>34</v>
       </c>
       <c r="F35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G35" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="4:12">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="4:12" x14ac:dyDescent="0.2">
       <c r="I36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J36" s="7" t="s">
         <v>20</v>
       </c>
       <c r="K36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L36" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="4:12">
+    <row r="37" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E37" t="s">
         <v>16</v>
       </c>
       <c r="F37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G37" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="4:12">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="4:12" x14ac:dyDescent="0.2">
       <c r="I38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J38" s="7" t="s">
         <v>36</v>
       </c>
       <c r="K38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L38" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="4:12">
+    <row r="39" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E39" t="s">
         <v>15</v>
       </c>
       <c r="F39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G39" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="40" spans="4:12">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="4:12" x14ac:dyDescent="0.2">
       <c r="I40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J40" s="10" t="s">
         <v>40</v>
       </c>
       <c r="K40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L40" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="4:12">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E41" t="s">
         <v>28</v>
       </c>
       <c r="F41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G41" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="4:12" ht="15.75">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="G42" s="9" t="s">
+        <v>68</v>
+      </c>
       <c r="I42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J42" s="13" t="s">
         <v>42</v>
       </c>
       <c r="K42" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L42" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="4:12">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E43" t="s">
         <v>8</v>
       </c>
       <c r="F43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G43" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="4:12">
+    <row r="44" spans="4:12" x14ac:dyDescent="0.2">
       <c r="I44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J44" t="s">
         <v>15</v>
       </c>
       <c r="K44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L44" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="45" spans="4:12">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E45" t="s">
         <v>29</v>
       </c>
       <c r="F45" t="s">
+        <v>61</v>
+      </c>
+      <c r="G45" t="s">
         <v>62</v>
       </c>
-      <c r="G45" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="46" spans="4:12">
+    </row>
+    <row r="46" spans="4:12" x14ac:dyDescent="0.2">
       <c r="G46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J46" t="s">
         <v>8</v>
       </c>
       <c r="K46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L46" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="4:12">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="4:12" x14ac:dyDescent="0.2">
       <c r="F47" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G47" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="4:12">
+    <row r="48" spans="4:12" x14ac:dyDescent="0.2">
       <c r="I48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J48" t="s">
         <v>29</v>
       </c>
       <c r="K48" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>